<commit_message>
Replaced try-catch and added new square APIs
</commit_message>
<xml_diff>
--- a/square_API_list.xlsx
+++ b/square_API_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\singer-tap\V2\tap-square\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125DBCB9-90E2-48C1-BD96-A678F80AB824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="111">
   <si>
     <t>Catalog</t>
   </si>
@@ -171,12 +172,198 @@
   </si>
   <si>
     <t>inventory_adjustment</t>
+  </si>
+  <si>
+    <t>API URL</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=category</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=discount</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=image</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=item</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=item_variation</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=modifier</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=modifier_list</t>
+  </si>
+  <si>
+    <t>v2/catalog/list?types=tax</t>
+  </si>
+  <si>
+    <t>v2/customers</t>
+  </si>
+  <si>
+    <t>v2/customers/{customer_id}</t>
+  </si>
+  <si>
+    <t>v2/inventory/batch-retrieve-changes</t>
+  </si>
+  <si>
+    <t>v2/inventory/batch-retrieve-counts</t>
+  </si>
+  <si>
+    <t>v2/employees</t>
+  </si>
+  <si>
+    <t>v2/employees/{id}</t>
+  </si>
+  <si>
+    <t>v2/labor/break-type</t>
+  </si>
+  <si>
+    <t>v2/labor/break-types/{id}</t>
+  </si>
+  <si>
+    <t>v2/labor/employee-wages</t>
+  </si>
+  <si>
+    <t>v2/labor/employee-wages/{id}</t>
+  </si>
+  <si>
+    <t>v2/labor/shifts/search</t>
+  </si>
+  <si>
+    <t>v2/labor/shifts/{id}</t>
+  </si>
+  <si>
+    <t>v2/labor/workweek-configs</t>
+  </si>
+  <si>
+    <t>v2/location</t>
+  </si>
+  <si>
+    <t>v2/locations/{location_id}</t>
+  </si>
+  <si>
+    <t>v2/merchants</t>
+  </si>
+  <si>
+    <t>v2/merchants/{merchant_id}</t>
+  </si>
+  <si>
+    <t>v2/customers/groups</t>
+  </si>
+  <si>
+    <t>v2/customers/groups/{group_id}</t>
+  </si>
+  <si>
+    <t>v2/customers/segments</t>
+  </si>
+  <si>
+    <t>v2/customers/segments/{segment_id}</t>
+  </si>
+  <si>
+    <t>v2/payments</t>
+  </si>
+  <si>
+    <t>v2/payments/{payment_id}</t>
+  </si>
+  <si>
+    <t>payment_id</t>
+  </si>
+  <si>
+    <t>v2/refunds</t>
+  </si>
+  <si>
+    <t>v2/refunds/{refund_id}</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>v2/orders/search</t>
+  </si>
+  <si>
+    <t>devices_codes</t>
+  </si>
+  <si>
+    <t>v2/devices/codes</t>
+  </si>
+  <si>
+    <t>retrieve_device_code</t>
+  </si>
+  <si>
+    <t>v2/devices/codes/{id}</t>
+  </si>
+  <si>
+    <t>retrieve_terminal_checkout</t>
+  </si>
+  <si>
+    <t>terminals_checkouts</t>
+  </si>
+  <si>
+    <t>v2/terminals/checkouts/search</t>
+  </si>
+  <si>
+    <t>v2/terminals/checkouts/{checkout_id}</t>
+  </si>
+  <si>
+    <t>checkout_id</t>
+  </si>
+  <si>
+    <t>refund_id</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>list_disputes</t>
+  </si>
+  <si>
+    <t>v2/disputes</t>
+  </si>
+  <si>
+    <t>retrieve_disputes</t>
+  </si>
+  <si>
+    <t>v2/disputes/{dispute_id}</t>
+  </si>
+  <si>
+    <t>dispute_id</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Refunds</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>Disputes</t>
+  </si>
+  <si>
+    <t>list_refunds</t>
+  </si>
+  <si>
+    <t>retrieve_payment</t>
+  </si>
+  <si>
+    <t>list_payments</t>
+  </si>
+  <si>
+    <t>retrieve_refund</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,12 +371,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -203,6 +384,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,17 +439,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,319 +734,560 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
+      <c r="C14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
+      <c r="C18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
+      <c r="C24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
+      <c r="C26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
+      <c r="C28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>